<commit_message>
by second testcasesssss,Comments by Admin a Test Sage User
</commit_message>
<xml_diff>
--- a/Excel/MyTestData.xlsx
+++ b/Excel/MyTestData.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -402,9 +402,25 @@
         <v>http://web.meehappy.com:9090/login</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>balrajhatti32@gmail.com</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Opal@123</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>sbasava022</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Opal@122</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>